<commit_message>
changed values due to new restaurant table
</commit_message>
<xml_diff>
--- a/FoodRecSVDTrain/kPlot.xlsx
+++ b/FoodRecSVDTrain/kPlot.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="19875" windowHeight="7710"/>
+    <workbookView xWindow="720" yWindow="645" windowWidth="19635" windowHeight="7425"/>
   </bookViews>
   <sheets>
     <sheet name="kPlot" sheetId="1" r:id="rId1"/>
@@ -598,10 +598,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>kPlot!$A$1:$A$147</c:f>
+              <c:f>kPlot!$A$1:$A$143</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="147"/>
+                <c:ptCount val="143"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1030,468 +1030,444 @@
                 </c:pt>
                 <c:pt idx="142">
                   <c:v>143</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>144</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>146</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>kPlot!$B$1:$B$147</c:f>
+              <c:f>kPlot!$B$1:$B$143</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="147"/>
+                <c:ptCount val="143"/>
                 <c:pt idx="0">
-                  <c:v>0.71105786463169396</c:v>
+                  <c:v>0.81569236961247904</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72510079890921497</c:v>
+                  <c:v>0.80666164936885199</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.67255075789118202</c:v>
+                  <c:v>0.71293423559965496</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.61149775502660098</c:v>
+                  <c:v>0.71808997802372299</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.60848519642987797</c:v>
+                  <c:v>0.66582334240128105</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59096161638563005</c:v>
+                  <c:v>0.67346753346577903</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.55187619413563405</c:v>
+                  <c:v>0.62572140068281901</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.53184637325072404</c:v>
+                  <c:v>0.60299145844410695</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52949086216934205</c:v>
+                  <c:v>0.58875656909873697</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.50942278103946503</c:v>
+                  <c:v>0.57366967392695001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.50399626903403305</c:v>
+                  <c:v>0.55265891706884196</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.48030245910808</c:v>
+                  <c:v>0.52586412534029803</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.46166199801006902</c:v>
+                  <c:v>0.51588743302862206</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.44364891292241798</c:v>
+                  <c:v>0.50738374799109098</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.41284278090311899</c:v>
+                  <c:v>0.48479151747931298</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.41541940008600298</c:v>
+                  <c:v>0.48606858645102502</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.398150666291119</c:v>
+                  <c:v>0.44401145539404802</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.37162821163260901</c:v>
+                  <c:v>0.42637301182956899</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.37224175058939801</c:v>
+                  <c:v>0.42564471226283301</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.37307048235041701</c:v>
+                  <c:v>0.406547446909239</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.35635001090707003</c:v>
+                  <c:v>0.40669888403479199</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.33642084077350798</c:v>
+                  <c:v>0.37703094738142701</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.33710495517845701</c:v>
+                  <c:v>0.39048040769054299</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.32458380688975302</c:v>
+                  <c:v>0.36200402854713798</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.31858627642371801</c:v>
+                  <c:v>0.36169707213112401</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.31321619151166002</c:v>
+                  <c:v>0.35411134129133798</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.29878027561762099</c:v>
+                  <c:v>0.33389642203689601</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.29737457206489898</c:v>
+                  <c:v>0.32739041417924702</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.28447394783404101</c:v>
+                  <c:v>0.317305753820537</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.27644921954643997</c:v>
+                  <c:v>0.30719489946314599</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.27674749109711599</c:v>
+                  <c:v>0.29069705447121702</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.262162246583869</c:v>
+                  <c:v>0.28808407448749201</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.24880130662708499</c:v>
+                  <c:v>0.29101423091991102</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.24598203818918099</c:v>
+                  <c:v>0.282887207708715</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.23307168004456699</c:v>
+                  <c:v>0.26106037856306402</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.235586459928327</c:v>
+                  <c:v>0.26231005594682399</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.22525102480304701</c:v>
+                  <c:v>0.25501453191652002</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.21564052121885899</c:v>
+                  <c:v>0.24772636554851299</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.21591434030576701</c:v>
+                  <c:v>0.240131291594191</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.20732415073737201</c:v>
+                  <c:v>0.23529516315389701</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.198768581530886</c:v>
+                  <c:v>0.23352834793885399</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.19998728162464099</c:v>
+                  <c:v>0.21789738535481301</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>0.19102006676684599</c:v>
+                  <c:v>0.21738330353720101</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.17833977881482299</c:v>
+                  <c:v>0.209388033155123</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.17788879056151299</c:v>
+                  <c:v>0.205915797777529</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.17503693605419501</c:v>
+                  <c:v>0.20144141760736201</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.163496357184747</c:v>
+                  <c:v>0.19643686644105501</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.161184072345467</c:v>
+                  <c:v>0.18900954994539501</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.155565715825419</c:v>
+                  <c:v>0.18388766320630801</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.153669529333606</c:v>
+                  <c:v>0.179504029179475</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.14961409652795701</c:v>
+                  <c:v>0.174007414417198</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.142784116639394</c:v>
+                  <c:v>0.16637480640302599</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.13548779781577</c:v>
+                  <c:v>0.16370043650004801</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.13473883087665001</c:v>
+                  <c:v>0.158410268059472</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.128800996759944</c:v>
+                  <c:v>0.14991054243163901</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.12418549414133701</c:v>
+                  <c:v>0.149444048892618</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.124715499742081</c:v>
+                  <c:v>0.14203288617152199</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.12072155433998701</c:v>
+                  <c:v>0.13572262462926099</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.11223734084763</c:v>
+                  <c:v>0.13210820017091399</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.105992035926328</c:v>
+                  <c:v>0.13040366372071499</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.105882266093456</c:v>
+                  <c:v>0.12669378053493399</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.101759291058934</c:v>
+                  <c:v>0.12147550116995801</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.10068094733267099</c:v>
+                  <c:v>0.116567700632353</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>9.8627243486599597E-2</c:v>
+                  <c:v>0.11379511152341</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>9.5342225080611298E-2</c:v>
+                  <c:v>0.10863853896870999</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>9.2166801439036397E-2</c:v>
+                  <c:v>0.102367685227294</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>8.7466583702139306E-2</c:v>
+                  <c:v>9.7670720235912098E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>8.3626046958004699E-2</c:v>
+                  <c:v>9.6233072193473407E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>8.1492643767668599E-2</c:v>
+                  <c:v>9.4485244940206797E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>7.9588664446820001E-2</c:v>
+                  <c:v>9.05258763001595E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>7.5940337311920805E-2</c:v>
+                  <c:v>8.7917200923025698E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>7.1835025031085895E-2</c:v>
+                  <c:v>8.6465945088275903E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>7.0851686598932206E-2</c:v>
+                  <c:v>7.8856756529268698E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>7.0017953761320195E-2</c:v>
+                  <c:v>7.5857765785668094E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>6.4690520000313501E-2</c:v>
+                  <c:v>7.5210176043008004E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>6.2431175302818498E-2</c:v>
+                  <c:v>7.2815304587615204E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>6.0587169882756101E-2</c:v>
+                  <c:v>6.9476574348271897E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>5.9196431576387397E-2</c:v>
+                  <c:v>6.7673081784623806E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>5.7917103623909803E-2</c:v>
+                  <c:v>6.5742279142541798E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>5.5659460845797398E-2</c:v>
+                  <c:v>6.2738521869155406E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5.3072376926229098E-2</c:v>
+                  <c:v>6.0439497388305397E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5.1125903619736499E-2</c:v>
+                  <c:v>5.8671715802160802E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.7013367514971302E-2</c:v>
+                  <c:v>5.4817007612753897E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.5679944100775603E-2</c:v>
+                  <c:v>5.3114479651266401E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.40066325201822E-2</c:v>
+                  <c:v>5.2467218365935098E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.1291912312114598E-2</c:v>
+                  <c:v>4.95446905220608E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>3.99722390788207E-2</c:v>
+                  <c:v>4.8794911362138399E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>3.8655897446965598E-2</c:v>
+                  <c:v>4.6524388034356698E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>3.7475321006695102E-2</c:v>
+                  <c:v>4.4614612860165902E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>3.5770652941081102E-2</c:v>
+                  <c:v>4.1417368691558001E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>3.3709220346369702E-2</c:v>
+                  <c:v>3.9858699795719398E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>3.2270618145977502E-2</c:v>
+                  <c:v>3.8304467668638202E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>3.1317718414707499E-2</c:v>
+                  <c:v>3.5473476182336101E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>3.0086136112238301E-2</c:v>
+                  <c:v>3.4196292085698701E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2.8951677244401199E-2</c:v>
+                  <c:v>3.3518070362395E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2.77819553769823E-2</c:v>
+                  <c:v>3.15091819333383E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.6985463420503002E-2</c:v>
+                  <c:v>2.9960115931097601E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.6026168046777799E-2</c:v>
+                  <c:v>2.8594836101025398E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.4921729729506899E-2</c:v>
+                  <c:v>2.76443961824312E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.42196959112242E-2</c:v>
+                  <c:v>2.6510249566591201E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.31090464198224E-2</c:v>
+                  <c:v>2.5707828029626002E-2</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.24510202432078E-2</c:v>
+                  <c:v>2.4476125362648201E-2</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.16651013803115E-2</c:v>
+                  <c:v>2.30557061324612E-2</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.0994774267439099E-2</c:v>
+                  <c:v>2.17696625331847E-2</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.01096174516497E-2</c:v>
+                  <c:v>2.0939397438554198E-2</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>1.8880617994793E-2</c:v>
+                  <c:v>2.0081370736600501E-2</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>1.78747713509783E-2</c:v>
+                  <c:v>1.9011868948944102E-2</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>1.69122858342854E-2</c:v>
+                  <c:v>1.8282957696402501E-2</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>1.6469529441893699E-2</c:v>
+                  <c:v>1.7243923157299199E-2</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>1.5999940864723301E-2</c:v>
+                  <c:v>1.6593325600238299E-2</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>1.5225978800572099E-2</c:v>
+                  <c:v>1.59510173881229E-2</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>1.45525381662146E-2</c:v>
+                  <c:v>1.5237597158361401E-2</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>1.37779497505423E-2</c:v>
+                  <c:v>1.4662207364773999E-2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>1.31127403709984E-2</c:v>
+                  <c:v>1.39605657735249E-2</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>1.22024684791867E-2</c:v>
+                  <c:v>1.2625273377709601E-2</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>1.14029293001817E-2</c:v>
+                  <c:v>1.1597681360417601E-2</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>1.0706882931999499E-2</c:v>
+                  <c:v>1.12340868533368E-2</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>9.9813067960865497E-3</c:v>
+                  <c:v>1.02947019964559E-2</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>9.33068983636718E-3</c:v>
+                  <c:v>9.7408840913035394E-3</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>8.6582290325050992E-3</c:v>
+                  <c:v>9.1482835617948399E-3</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>8.4440708506741905E-3</c:v>
+                  <c:v>8.5646561508695099E-3</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>7.9335554107207197E-3</c:v>
+                  <c:v>8.1175503754009008E-3</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>7.5359346505659503E-3</c:v>
+                  <c:v>7.3883400714864602E-3</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>7.03064042812302E-3</c:v>
+                  <c:v>6.75380431956084E-3</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>6.5770948213708502E-3</c:v>
+                  <c:v>6.12371917656215E-3</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>6.2150836524568999E-3</c:v>
+                  <c:v>5.5793857622041202E-3</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>5.9535598991725504E-3</c:v>
+                  <c:v>4.7246603287597602E-3</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>5.6863044218854299E-3</c:v>
+                  <c:v>3.98892023380641E-3</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>5.01104292968682E-3</c:v>
+                  <c:v>3.5328964446700701E-3</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>4.4463541176767499E-3</c:v>
+                  <c:v>2.92232547765915E-3</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>4.0662190105232102E-3</c:v>
+                  <c:v>2.49497506454225E-3</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>3.5564760796511301E-3</c:v>
+                  <c:v>1.9801115841158699E-3</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>2.9954334214214E-3</c:v>
+                  <c:v>1.7385326628395301E-3</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>2.7436053673234001E-3</c:v>
+                  <c:v>1.5727484616869999E-3</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>2.3235601178124001E-3</c:v>
+                  <c:v>1.3429853761654099E-3</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>1.9909152886012599E-3</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1.74596252651346E-3</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>1.55640908251593E-3</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>1.3768455869965801E-3</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>1.08122124341781E-3</c:v>
+                  <c:v>1.0673344509293801E-3</c:v>
+                </c:pt>
+                <c:pt idx="136" formatCode="0.00E+00">
+                  <c:v>9.3075965113281398E-4</c:v>
+                </c:pt>
+                <c:pt idx="137" formatCode="0.00E+00">
+                  <c:v>6.9990658632283298E-4</c:v>
+                </c:pt>
+                <c:pt idx="138" formatCode="0.00E+00">
+                  <c:v>4.4118754297899201E-4</c:v>
+                </c:pt>
+                <c:pt idx="139" formatCode="0.00E+00">
+                  <c:v>2.3381861074141201E-4</c:v>
                 </c:pt>
                 <c:pt idx="140" formatCode="0.00E+00">
-                  <c:v>8.8922098581825301E-4</c:v>
+                  <c:v>1.00692228266394E-4</c:v>
                 </c:pt>
                 <c:pt idx="141" formatCode="0.00E+00">
-                  <c:v>6.0934345768945105E-4</c:v>
+                  <c:v>4.2361860653732299E-5</c:v>
                 </c:pt>
                 <c:pt idx="142" formatCode="0.00E+00">
-                  <c:v>3.7300109653881901E-4</c:v>
-                </c:pt>
-                <c:pt idx="143" formatCode="0.00E+00">
-                  <c:v>2.4926324087951902E-4</c:v>
-                </c:pt>
-                <c:pt idx="144" formatCode="0.00E+00">
-                  <c:v>1.55846086876805E-4</c:v>
-                </c:pt>
-                <c:pt idx="145" formatCode="0.00E+00">
-                  <c:v>5.5167495991488897E-5</c:v>
-                </c:pt>
-                <c:pt idx="146" formatCode="0.00E+00">
-                  <c:v>1.1056728784233799E-5</c:v>
+                  <c:v>1.2024591867074899E-5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,11 +1482,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="52359552"/>
-        <c:axId val="72569984"/>
+        <c:axId val="96111232"/>
+        <c:axId val="96109696"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52359552"/>
+        <c:axId val="96111232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,12 +1515,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72569984"/>
+        <c:crossAx val="96109696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72569984"/>
+        <c:axId val="96109696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,7 +1550,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52359552"/>
+        <c:crossAx val="96111232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1913,11 +1889,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B147"/>
+  <dimension ref="A1:B143"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1926,7 +1900,7 @@
         <v>1</v>
       </c>
       <c r="B1">
-        <v>0.71105786463169396</v>
+        <v>0.81569236961247904</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1934,7 +1908,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.72510079890921497</v>
+        <v>0.80666164936885199</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1942,7 +1916,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.67255075789118202</v>
+        <v>0.71293423559965496</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1950,7 +1924,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.61149775502660098</v>
+        <v>0.71808997802372299</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1958,7 +1932,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.60848519642987797</v>
+        <v>0.66582334240128105</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1966,7 +1940,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.59096161638563005</v>
+        <v>0.67346753346577903</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1974,7 +1948,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.55187619413563405</v>
+        <v>0.62572140068281901</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1982,7 +1956,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.53184637325072404</v>
+        <v>0.60299145844410695</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,7 +1964,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.52949086216934205</v>
+        <v>0.58875656909873697</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1998,7 +1972,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.50942278103946503</v>
+        <v>0.57366967392695001</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -2006,7 +1980,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.50399626903403305</v>
+        <v>0.55265891706884196</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -2014,7 +1988,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.48030245910808</v>
+        <v>0.52586412534029803</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -2022,7 +1996,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.46166199801006902</v>
+        <v>0.51588743302862206</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -2030,7 +2004,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.44364891292241798</v>
+        <v>0.50738374799109098</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -2038,7 +2012,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.41284278090311899</v>
+        <v>0.48479151747931298</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -2046,7 +2020,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.41541940008600298</v>
+        <v>0.48606858645102502</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -2054,7 +2028,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.398150666291119</v>
+        <v>0.44401145539404802</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -2062,7 +2036,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.37162821163260901</v>
+        <v>0.42637301182956899</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -2070,7 +2044,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.37224175058939801</v>
+        <v>0.42564471226283301</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -2078,7 +2052,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.37307048235041701</v>
+        <v>0.406547446909239</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -2086,7 +2060,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>0.35635001090707003</v>
+        <v>0.40669888403479199</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -2094,7 +2068,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>0.33642084077350798</v>
+        <v>0.37703094738142701</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -2102,7 +2076,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>0.33710495517845701</v>
+        <v>0.39048040769054299</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -2110,7 +2084,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>0.32458380688975302</v>
+        <v>0.36200402854713798</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -2118,7 +2092,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>0.31858627642371801</v>
+        <v>0.36169707213112401</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -2126,7 +2100,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>0.31321619151166002</v>
+        <v>0.35411134129133798</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -2134,7 +2108,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>0.29878027561762099</v>
+        <v>0.33389642203689601</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -2142,7 +2116,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>0.29737457206489898</v>
+        <v>0.32739041417924702</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -2150,7 +2124,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>0.28447394783404101</v>
+        <v>0.317305753820537</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -2158,7 +2132,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>0.27644921954643997</v>
+        <v>0.30719489946314599</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -2166,7 +2140,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>0.27674749109711599</v>
+        <v>0.29069705447121702</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -2174,7 +2148,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>0.262162246583869</v>
+        <v>0.28808407448749201</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2182,7 +2156,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>0.24880130662708499</v>
+        <v>0.29101423091991102</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -2190,7 +2164,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>0.24598203818918099</v>
+        <v>0.282887207708715</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2198,7 +2172,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>0.23307168004456699</v>
+        <v>0.26106037856306402</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2206,7 +2180,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>0.235586459928327</v>
+        <v>0.26231005594682399</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2214,7 +2188,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>0.22525102480304701</v>
+        <v>0.25501453191652002</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -2222,7 +2196,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>0.21564052121885899</v>
+        <v>0.24772636554851299</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -2230,7 +2204,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>0.21591434030576701</v>
+        <v>0.240131291594191</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -2238,7 +2212,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>0.20732415073737201</v>
+        <v>0.23529516315389701</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -2246,7 +2220,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>0.198768581530886</v>
+        <v>0.23352834793885399</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -2254,7 +2228,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>0.19998728162464099</v>
+        <v>0.21789738535481301</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -2262,7 +2236,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>0.19102006676684599</v>
+        <v>0.21738330353720101</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2270,7 +2244,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>0.17833977881482299</v>
+        <v>0.209388033155123</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2278,7 +2252,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>0.17788879056151299</v>
+        <v>0.205915797777529</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2286,7 +2260,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>0.17503693605419501</v>
+        <v>0.20144141760736201</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2294,7 +2268,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>0.163496357184747</v>
+        <v>0.19643686644105501</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2302,7 +2276,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>0.161184072345467</v>
+        <v>0.18900954994539501</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2310,7 +2284,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>0.155565715825419</v>
+        <v>0.18388766320630801</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2318,7 +2292,7 @@
         <v>50</v>
       </c>
       <c r="B50">
-        <v>0.153669529333606</v>
+        <v>0.179504029179475</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2326,7 +2300,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>0.14961409652795701</v>
+        <v>0.174007414417198</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2334,7 +2308,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>0.142784116639394</v>
+        <v>0.16637480640302599</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2342,7 +2316,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>0.13548779781577</v>
+        <v>0.16370043650004801</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2350,7 +2324,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>0.13473883087665001</v>
+        <v>0.158410268059472</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2358,7 +2332,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>0.128800996759944</v>
+        <v>0.14991054243163901</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2366,7 +2340,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>0.12418549414133701</v>
+        <v>0.149444048892618</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2374,7 +2348,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>0.124715499742081</v>
+        <v>0.14203288617152199</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2382,7 +2356,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>0.12072155433998701</v>
+        <v>0.13572262462926099</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2390,7 +2364,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>0.11223734084763</v>
+        <v>0.13210820017091399</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2398,7 +2372,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>0.105992035926328</v>
+        <v>0.13040366372071499</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2406,7 +2380,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>0.105882266093456</v>
+        <v>0.12669378053493399</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2414,7 +2388,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>0.101759291058934</v>
+        <v>0.12147550116995801</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2422,7 +2396,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>0.10068094733267099</v>
+        <v>0.116567700632353</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2430,7 +2404,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>9.8627243486599597E-2</v>
+        <v>0.11379511152341</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2438,7 +2412,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>9.5342225080611298E-2</v>
+        <v>0.10863853896870999</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2446,7 +2420,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>9.2166801439036397E-2</v>
+        <v>0.102367685227294</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2454,7 +2428,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>8.7466583702139306E-2</v>
+        <v>9.7670720235912098E-2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2462,7 +2436,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>8.3626046958004699E-2</v>
+        <v>9.6233072193473407E-2</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2470,7 +2444,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>8.1492643767668599E-2</v>
+        <v>9.4485244940206797E-2</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2478,7 +2452,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>7.9588664446820001E-2</v>
+        <v>9.05258763001595E-2</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2486,7 +2460,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>7.5940337311920805E-2</v>
+        <v>8.7917200923025698E-2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +2468,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>7.1835025031085895E-2</v>
+        <v>8.6465945088275903E-2</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2476,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>7.0851686598932206E-2</v>
+        <v>7.8856756529268698E-2</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2510,7 +2484,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>7.0017953761320195E-2</v>
+        <v>7.5857765785668094E-2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2518,7 +2492,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>6.4690520000313501E-2</v>
+        <v>7.5210176043008004E-2</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2526,7 +2500,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>6.2431175302818498E-2</v>
+        <v>7.2815304587615204E-2</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2534,7 +2508,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>6.0587169882756101E-2</v>
+        <v>6.9476574348271897E-2</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2542,7 +2516,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>5.9196431576387397E-2</v>
+        <v>6.7673081784623806E-2</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2550,7 +2524,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>5.7917103623909803E-2</v>
+        <v>6.5742279142541798E-2</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2558,7 +2532,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>5.5659460845797398E-2</v>
+        <v>6.2738521869155406E-2</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2566,7 +2540,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>5.3072376926229098E-2</v>
+        <v>6.0439497388305397E-2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2574,7 +2548,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>5.1125903619736499E-2</v>
+        <v>5.8671715802160802E-2</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2582,7 +2556,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>4.7013367514971302E-2</v>
+        <v>5.4817007612753897E-2</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2590,7 +2564,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>4.5679944100775603E-2</v>
+        <v>5.3114479651266401E-2</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2598,7 +2572,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>4.40066325201822E-2</v>
+        <v>5.2467218365935098E-2</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2606,7 +2580,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>4.1291912312114598E-2</v>
+        <v>4.95446905220608E-2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2614,7 +2588,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>3.99722390788207E-2</v>
+        <v>4.8794911362138399E-2</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2622,7 +2596,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>3.8655897446965598E-2</v>
+        <v>4.6524388034356698E-2</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2630,7 +2604,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>3.7475321006695102E-2</v>
+        <v>4.4614612860165902E-2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2638,7 +2612,7 @@
         <v>90</v>
       </c>
       <c r="B90">
-        <v>3.5770652941081102E-2</v>
+        <v>4.1417368691558001E-2</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2646,7 +2620,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>3.3709220346369702E-2</v>
+        <v>3.9858699795719398E-2</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2654,7 +2628,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>3.2270618145977502E-2</v>
+        <v>3.8304467668638202E-2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2662,7 +2636,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>3.1317718414707499E-2</v>
+        <v>3.5473476182336101E-2</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2670,7 +2644,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>3.0086136112238301E-2</v>
+        <v>3.4196292085698701E-2</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2678,7 +2652,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>2.8951677244401199E-2</v>
+        <v>3.3518070362395E-2</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2686,7 +2660,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>2.77819553769823E-2</v>
+        <v>3.15091819333383E-2</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2694,7 +2668,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>2.6985463420503002E-2</v>
+        <v>2.9960115931097601E-2</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2702,7 +2676,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>2.6026168046777799E-2</v>
+        <v>2.8594836101025398E-2</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2710,7 +2684,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>2.4921729729506899E-2</v>
+        <v>2.76443961824312E-2</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2718,7 +2692,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>2.42196959112242E-2</v>
+        <v>2.6510249566591201E-2</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2726,7 +2700,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>2.31090464198224E-2</v>
+        <v>2.5707828029626002E-2</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2734,7 +2708,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>2.24510202432078E-2</v>
+        <v>2.4476125362648201E-2</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2742,7 +2716,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>2.16651013803115E-2</v>
+        <v>2.30557061324612E-2</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2750,7 +2724,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>2.0994774267439099E-2</v>
+        <v>2.17696625331847E-2</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2758,7 +2732,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>2.01096174516497E-2</v>
+        <v>2.0939397438554198E-2</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2766,7 +2740,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>1.8880617994793E-2</v>
+        <v>2.0081370736600501E-2</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2774,7 +2748,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>1.78747713509783E-2</v>
+        <v>1.9011868948944102E-2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2782,7 +2756,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>1.69122858342854E-2</v>
+        <v>1.8282957696402501E-2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2790,7 +2764,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>1.6469529441893699E-2</v>
+        <v>1.7243923157299199E-2</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2798,7 +2772,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>1.5999940864723301E-2</v>
+        <v>1.6593325600238299E-2</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2806,7 +2780,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>1.5225978800572099E-2</v>
+        <v>1.59510173881229E-2</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2814,7 +2788,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>1.45525381662146E-2</v>
+        <v>1.5237597158361401E-2</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2822,7 +2796,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>1.37779497505423E-2</v>
+        <v>1.4662207364773999E-2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2830,7 +2804,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>1.31127403709984E-2</v>
+        <v>1.39605657735249E-2</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2838,7 +2812,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>1.22024684791867E-2</v>
+        <v>1.2625273377709601E-2</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2846,7 +2820,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>1.14029293001817E-2</v>
+        <v>1.1597681360417601E-2</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2854,7 +2828,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>1.0706882931999499E-2</v>
+        <v>1.12340868533368E-2</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2862,7 +2836,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>9.9813067960865497E-3</v>
+        <v>1.02947019964559E-2</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2870,7 +2844,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>9.33068983636718E-3</v>
+        <v>9.7408840913035394E-3</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2878,7 +2852,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>8.6582290325050992E-3</v>
+        <v>9.1482835617948399E-3</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2886,7 +2860,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>8.4440708506741905E-3</v>
+        <v>8.5646561508695099E-3</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2894,7 +2868,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>7.9335554107207197E-3</v>
+        <v>8.1175503754009008E-3</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2902,7 +2876,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>7.5359346505659503E-3</v>
+        <v>7.3883400714864602E-3</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2910,7 +2884,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>7.03064042812302E-3</v>
+        <v>6.75380431956084E-3</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2918,7 +2892,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>6.5770948213708502E-3</v>
+        <v>6.12371917656215E-3</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2926,7 +2900,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>6.2150836524568999E-3</v>
+        <v>5.5793857622041202E-3</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2934,7 +2908,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>5.9535598991725504E-3</v>
+        <v>4.7246603287597602E-3</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2942,7 +2916,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>5.6863044218854299E-3</v>
+        <v>3.98892023380641E-3</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2950,7 +2924,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>5.01104292968682E-3</v>
+        <v>3.5328964446700701E-3</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
@@ -2958,7 +2932,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>4.4463541176767499E-3</v>
+        <v>2.92232547765915E-3</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
@@ -2966,7 +2940,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>4.0662190105232102E-3</v>
+        <v>2.49497506454225E-3</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
@@ -2974,7 +2948,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>3.5564760796511301E-3</v>
+        <v>1.9801115841158699E-3</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
@@ -2982,7 +2956,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>2.9954334214214E-3</v>
+        <v>1.7385326628395301E-3</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
@@ -2990,7 +2964,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>2.7436053673234001E-3</v>
+        <v>1.5727484616869999E-3</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
@@ -2998,7 +2972,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>2.3235601178124001E-3</v>
+        <v>1.3429853761654099E-3</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
@@ -3006,39 +2980,39 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>1.9909152886012599E-3</v>
+        <v>1.0673344509293801E-3</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>137</v>
       </c>
-      <c r="B137">
-        <v>1.74596252651346E-3</v>
+      <c r="B137" s="1">
+        <v>9.3075965113281398E-4</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>138</v>
       </c>
-      <c r="B138">
-        <v>1.55640908251593E-3</v>
+      <c r="B138" s="1">
+        <v>6.9990658632283298E-4</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>139</v>
       </c>
-      <c r="B139">
-        <v>1.3768455869965801E-3</v>
+      <c r="B139" s="1">
+        <v>4.4118754297899201E-4</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>140</v>
       </c>
-      <c r="B140">
-        <v>1.08122124341781E-3</v>
+      <c r="B140" s="1">
+        <v>2.3381861074141201E-4</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
@@ -3046,7 +3020,7 @@
         <v>141</v>
       </c>
       <c r="B141" s="1">
-        <v>8.8922098581825301E-4</v>
+        <v>1.00692228266394E-4</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
@@ -3054,7 +3028,7 @@
         <v>142</v>
       </c>
       <c r="B142" s="1">
-        <v>6.0934345768945105E-4</v>
+        <v>4.2361860653732299E-5</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
@@ -3062,39 +3036,7 @@
         <v>143</v>
       </c>
       <c r="B143" s="1">
-        <v>3.7300109653881901E-4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144">
-        <v>144</v>
-      </c>
-      <c r="B144" s="1">
-        <v>2.4926324087951902E-4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145">
-        <v>145</v>
-      </c>
-      <c r="B145" s="1">
-        <v>1.55846086876805E-4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146">
-        <v>146</v>
-      </c>
-      <c r="B146" s="1">
-        <v>5.5167495991488897E-5</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147">
-        <v>147</v>
-      </c>
-      <c r="B147" s="1">
-        <v>1.1056728784233799E-5</v>
+        <v>1.2024591867074899E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>